<commit_message>
update data scientist skill
</commit_message>
<xml_diff>
--- a/Personal/data_scientist_skills_list.xlsx
+++ b/Personal/data_scientist_skills_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HDENG\Documents\github\documents\Personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdeng\Documents\GitHub\documents\Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" xr2:uid="{A99FE088-F06D-4AB1-9386-5848590ACF85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13640" xr2:uid="{A99FE088-F06D-4AB1-9386-5848590ACF85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="192">
   <si>
     <t>fundamentals</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -406,14 +406,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Logiistic regression</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rankking</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Linear Regression</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -788,6 +780,15 @@
   <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tried</t>
+  </si>
+  <si>
+    <t>Logisitic regression</t>
+  </si>
+  <si>
+    <t>Ranking</t>
   </si>
 </sst>
 </file>
@@ -798,14 +799,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -814,7 +815,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -844,10 +845,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1164,31 +1165,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896067B0-39D2-47CC-9E33-4B4BFF4A5860}">
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.125" customWidth="1"/>
-    <col min="2" max="2" width="44.375" customWidth="1"/>
+    <col min="1" max="1" width="25.08984375" customWidth="1"/>
+    <col min="2" max="2" width="44.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1196,109 +1197,109 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B20" t="s">
@@ -1306,175 +1307,175 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
       <c r="B21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
       <c r="B22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
       <c r="B25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2"/>
       <c r="B29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
       <c r="B31" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
       <c r="B32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2"/>
       <c r="B33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1"/>
+      <c r="A34" s="2"/>
       <c r="B34" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1"/>
+      <c r="A35" s="2"/>
       <c r="B35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="1"/>
+      <c r="A36" s="2"/>
       <c r="B36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="1"/>
+      <c r="A37" s="2"/>
       <c r="B37" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2"/>
       <c r="B38" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="1"/>
+      <c r="A39" s="2"/>
       <c r="B39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="1"/>
+      <c r="A40" s="2"/>
       <c r="B40" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2"/>
       <c r="B41" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2"/>
       <c r="B42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="1"/>
+      <c r="A43" s="2"/>
       <c r="B43" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1"/>
+      <c r="A44" s="2"/>
       <c r="B44" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="1"/>
+      <c r="A45" s="2"/>
       <c r="B45" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="2"/>
       <c r="B46" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="2"/>
       <c r="B47" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="1"/>
+      <c r="A48" s="2"/>
       <c r="B48" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B49" t="s">
@@ -1482,133 +1483,133 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="1"/>
+      <c r="A50" s="2"/>
       <c r="B50" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="1"/>
+      <c r="A51" s="2"/>
       <c r="B51" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="1"/>
+      <c r="A52" s="2"/>
       <c r="B52" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="1"/>
+      <c r="A53" s="2"/>
       <c r="B53" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="1"/>
+      <c r="A54" s="2"/>
       <c r="B54" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="1"/>
+      <c r="A55" s="2"/>
       <c r="B55" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="1"/>
+      <c r="A56" s="2"/>
       <c r="B56" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="1"/>
+      <c r="A57" s="2"/>
       <c r="B57" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="1"/>
+      <c r="A58" s="2"/>
       <c r="B58" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="1"/>
+      <c r="A59" s="2"/>
       <c r="B59" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="1"/>
+      <c r="A60" s="2"/>
       <c r="B60" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="1"/>
+      <c r="A61" s="2"/>
       <c r="B61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="1"/>
+      <c r="A62" s="2"/>
       <c r="B62" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="1"/>
+      <c r="A63" s="2"/>
       <c r="B63" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="1"/>
+      <c r="A64" s="2"/>
       <c r="B64" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="1"/>
+      <c r="A65" s="2"/>
       <c r="B65" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="2"/>
       <c r="B66" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="1"/>
+      <c r="A67" s="2"/>
       <c r="B67" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="1"/>
+      <c r="A68" s="2"/>
       <c r="B68" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="1"/>
+      <c r="A69" s="2"/>
       <c r="B69" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="1"/>
+      <c r="A70" s="2"/>
       <c r="B70" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B71" t="s">
@@ -1616,701 +1617,719 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="2"/>
       <c r="B72" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="1"/>
+      <c r="A73" s="2"/>
       <c r="B73" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1"/>
+      <c r="A74" s="2"/>
       <c r="B74" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="1"/>
+      <c r="A75" s="2"/>
       <c r="B75" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="1"/>
+      <c r="A76" s="2"/>
       <c r="B76" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="1"/>
+      <c r="A77" s="2"/>
       <c r="B77" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="1"/>
+      <c r="A78" s="2"/>
       <c r="B78" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="1"/>
+      <c r="A79" s="2"/>
       <c r="B79" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="1"/>
+      <c r="A80" s="2"/>
       <c r="B80" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1"/>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2"/>
       <c r="B81" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1"/>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2"/>
       <c r="B82" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1"/>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2"/>
       <c r="B83" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1"/>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2"/>
       <c r="B84" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="1"/>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2"/>
       <c r="B85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="1"/>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2"/>
       <c r="B86" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="1"/>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2"/>
       <c r="B87" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="1"/>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2"/>
       <c r="B88" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="1"/>
+      <c r="C88" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2"/>
       <c r="B89" t="s">
+        <v>109</v>
+      </c>
+      <c r="C89" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2"/>
+      <c r="B90" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2"/>
+      <c r="B91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2"/>
+      <c r="B92" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="1"/>
-      <c r="B90" t="s">
+      <c r="C92" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2"/>
+      <c r="B93" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="1"/>
-      <c r="B91" t="s">
+    <row r="94" spans="1:3">
+      <c r="A94" s="2"/>
+      <c r="B94" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="1"/>
-      <c r="B92" t="s">
+    <row r="95" spans="1:3">
+      <c r="A95" s="2"/>
+      <c r="B95" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="1"/>
-      <c r="B93" t="s">
+      <c r="C95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2"/>
+      <c r="B96" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="1"/>
-      <c r="B94" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="2"/>
+      <c r="B97" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="1"/>
-      <c r="B95" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="2"/>
+      <c r="B98" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="1"/>
-      <c r="B96" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="2"/>
+      <c r="B99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="1"/>
-      <c r="B97" t="s">
+    <row r="100" spans="1:2">
+      <c r="A100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="1"/>
-      <c r="B98" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" s="2"/>
+      <c r="B101" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" s="2"/>
+      <c r="B102" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="1"/>
-      <c r="B100" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" s="2"/>
+      <c r="B103" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="1"/>
-      <c r="B101" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" s="2"/>
+      <c r="B104" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="1"/>
-      <c r="B102" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" s="2"/>
+      <c r="B105" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="1"/>
-      <c r="B103" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" s="2"/>
+      <c r="B106" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="1"/>
-      <c r="B104" t="s">
+    <row r="107" spans="1:2">
+      <c r="A107" s="2"/>
+      <c r="B107" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="1"/>
-      <c r="B105" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" s="2"/>
+      <c r="B108" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="1"/>
-      <c r="B106" t="s">
+    <row r="109" spans="1:2">
+      <c r="A109" s="2"/>
+      <c r="B109" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="1"/>
-      <c r="B107" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" s="2"/>
+      <c r="B110" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2"/>
+      <c r="B111" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="2"/>
+      <c r="B112" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="2"/>
+      <c r="B113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="2"/>
+      <c r="B114" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="2"/>
+      <c r="B116" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="2"/>
+      <c r="B117" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="2"/>
+      <c r="B118" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="2"/>
+      <c r="B119" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="2"/>
+      <c r="B120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="2"/>
+      <c r="B121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="2"/>
+      <c r="B122" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="2"/>
+      <c r="B123" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="2"/>
+      <c r="B124" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="2"/>
+      <c r="B125" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="2"/>
+      <c r="B126" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="2"/>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="2"/>
+      <c r="B128" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="2"/>
+      <c r="B129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B130" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="2"/>
+      <c r="B131" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="2"/>
+      <c r="B132" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="2"/>
+      <c r="B133" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="2"/>
+      <c r="B134" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="2"/>
+      <c r="B135" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="2"/>
+      <c r="B136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="2"/>
+      <c r="B137" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="2"/>
+      <c r="B138" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="2"/>
+      <c r="B139" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="2"/>
+      <c r="B140" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="2"/>
+      <c r="B141" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="2"/>
+      <c r="B142" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="2"/>
+      <c r="B143" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1"/>
-      <c r="B108" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="1"/>
-      <c r="B109" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="1"/>
-      <c r="B110" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="1"/>
-      <c r="B111" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1"/>
-      <c r="B112" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="1"/>
-      <c r="B113" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B114" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="1"/>
-      <c r="B115" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="1"/>
-      <c r="B116" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="1"/>
-      <c r="B117" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="1"/>
-      <c r="B118" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="1"/>
-      <c r="B119" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="1"/>
-      <c r="B120" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="1"/>
-      <c r="B121" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="1"/>
-      <c r="B122" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="1"/>
-      <c r="B123" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="1"/>
-      <c r="B124" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="1"/>
-      <c r="B125" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="1"/>
-      <c r="B126" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="1"/>
-      <c r="B127" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="1"/>
-      <c r="B128" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B129" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="1"/>
-      <c r="B130" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="1"/>
-      <c r="B131" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="1"/>
-      <c r="B132" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="1"/>
-      <c r="B133" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="1"/>
-      <c r="B134" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="1"/>
-      <c r="B135" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="1"/>
-      <c r="B136" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="1"/>
-      <c r="B137" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="1"/>
-      <c r="B138" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="1"/>
-      <c r="B139" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="1"/>
-      <c r="B140" t="s">
+    <row r="144" spans="1:2">
+      <c r="A144" s="2"/>
+      <c r="B144" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="1"/>
-      <c r="B141" t="s">
+    <row r="145" spans="1:2">
+      <c r="A145" s="2"/>
+      <c r="B145" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="1"/>
-      <c r="B142" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="1"/>
-      <c r="B143" t="s">
+    <row r="146" spans="1:2">
+      <c r="A146" s="2"/>
+      <c r="B146" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="1"/>
-      <c r="B144" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" s="2"/>
+      <c r="B147" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="1"/>
-      <c r="B145" t="s">
+    <row r="148" spans="1:2">
+      <c r="A148" s="2"/>
+      <c r="B148" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="1"/>
-      <c r="B146" t="s">
+    <row r="149" spans="1:2">
+      <c r="A149" s="2"/>
+      <c r="B149" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="1"/>
-      <c r="B147" t="s">
+    <row r="150" spans="1:2">
+      <c r="A150" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B150" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="1"/>
-      <c r="B148" t="s">
+    <row r="151" spans="1:2">
+      <c r="A151" s="2"/>
+      <c r="B151" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B149" t="s">
+    <row r="152" spans="1:2">
+      <c r="A152" s="2"/>
+      <c r="B152" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="1"/>
-      <c r="B150" t="s">
+    <row r="153" spans="1:2">
+      <c r="A153" s="2"/>
+      <c r="B153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="2"/>
+      <c r="B154" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="2"/>
+      <c r="B155" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="2"/>
+      <c r="B156" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="2"/>
+      <c r="B157" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="2"/>
+      <c r="B158" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="2"/>
+      <c r="B159" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="2"/>
+      <c r="B161" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="2"/>
+      <c r="B162" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="2"/>
+      <c r="B163" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="1"/>
-      <c r="B151" t="s">
+    <row r="164" spans="1:2">
+      <c r="A164" s="2"/>
+      <c r="B164" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="1"/>
-      <c r="B152" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="1"/>
-      <c r="B153" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="1"/>
-      <c r="B154" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="1"/>
-      <c r="B155" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="1"/>
-      <c r="B156" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="1"/>
-      <c r="B157" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="1"/>
-      <c r="B158" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B159" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="1"/>
-      <c r="B160" t="s">
+    <row r="165" spans="1:2">
+      <c r="A165" s="2"/>
+      <c r="B165" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="1"/>
-      <c r="B161" t="s">
+    <row r="166" spans="1:2">
+      <c r="A166" s="2"/>
+      <c r="B166" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="2"/>
+      <c r="B167" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="1"/>
-      <c r="B162" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="1"/>
-      <c r="B163" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" s="1"/>
-      <c r="B164" t="s">
+    <row r="168" spans="1:2">
+      <c r="A168" s="2"/>
+      <c r="B168" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
-      <c r="A165" s="1"/>
-      <c r="B165" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166" s="1"/>
-      <c r="B166" t="s">
+    <row r="169" spans="1:2">
+      <c r="A169" s="2"/>
+      <c r="B169" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
-      <c r="A167" s="1"/>
-      <c r="B167" t="s">
+    <row r="170" spans="1:2">
+      <c r="A170" s="2"/>
+      <c r="B170" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
-      <c r="A168" s="1"/>
-      <c r="B168" t="s">
+    <row r="171" spans="1:2">
+      <c r="A171" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B171" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
-      <c r="A169" s="1"/>
-      <c r="B169" t="s">
+    <row r="172" spans="1:2">
+      <c r="A172" s="2"/>
+      <c r="B172" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
-      <c r="A170" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B170" t="s">
+    <row r="173" spans="1:2">
+      <c r="A173" s="2"/>
+      <c r="B173" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
-      <c r="A171" s="1"/>
-      <c r="B171" t="s">
+    <row r="174" spans="1:2">
+      <c r="A174" s="2"/>
+      <c r="B174" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
-      <c r="A172" s="1"/>
-      <c r="B172" t="s">
+    <row r="175" spans="1:2">
+      <c r="A175" s="2"/>
+      <c r="B175" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
-      <c r="A173" s="1"/>
-      <c r="B173" t="s">
+    <row r="176" spans="1:2">
+      <c r="A176" s="2"/>
+      <c r="B176" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174" s="1"/>
-      <c r="B174" t="s">
+    <row r="177" spans="1:2">
+      <c r="A177" s="2"/>
+      <c r="B177" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
-      <c r="A175" s="1"/>
-      <c r="B175" t="s">
+    <row r="178" spans="1:2">
+      <c r="A178" s="2"/>
+      <c r="B178" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
-      <c r="A176" s="1"/>
-      <c r="B176" t="s">
+    <row r="179" spans="1:2">
+      <c r="A179" s="2"/>
+      <c r="B179" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
-      <c r="A177" s="1"/>
-      <c r="B177" t="s">
+    <row r="180" spans="1:2">
+      <c r="A180" s="2"/>
+      <c r="B180" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
-      <c r="A178" s="1"/>
-      <c r="B178" t="s">
+    <row r="181" spans="1:2">
+      <c r="A181" s="2"/>
+      <c r="B181" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
-      <c r="A179" s="1"/>
-      <c r="B179" t="s">
+    <row r="182" spans="1:2">
+      <c r="A182" s="2"/>
+      <c r="B182" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
-      <c r="A180" s="1"/>
-      <c r="B180" t="s">
+    <row r="183" spans="1:2">
+      <c r="A183" s="2"/>
+      <c r="B183" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
-      <c r="A181" s="1"/>
-      <c r="B181" t="s">
+    <row r="184" spans="1:2">
+      <c r="A184" s="2"/>
+      <c r="B184" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
-      <c r="A182" s="1"/>
-      <c r="B182" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
-      <c r="A183" s="1"/>
-      <c r="B183" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A129:A148"/>
-    <mergeCell ref="A149:A158"/>
-    <mergeCell ref="A159:A169"/>
-    <mergeCell ref="A170:A183"/>
+    <mergeCell ref="A130:A149"/>
+    <mergeCell ref="A150:A159"/>
+    <mergeCell ref="A160:A170"/>
+    <mergeCell ref="A171:A184"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A48"/>
     <mergeCell ref="A49:A70"/>
-    <mergeCell ref="A71:A98"/>
-    <mergeCell ref="A99:A113"/>
-    <mergeCell ref="A114:A128"/>
+    <mergeCell ref="A71:A99"/>
+    <mergeCell ref="A100:A114"/>
+    <mergeCell ref="A115:A129"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>